<commit_message>
cap nhat tai lieu - 220915
</commit_message>
<xml_diff>
--- a/Manufacture/BoM.xlsx
+++ b/Manufacture/BoM.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="408" windowWidth="14352" windowHeight="7380" activeTab="2"/>
+    <workbookView xWindow="480" yWindow="408" windowWidth="14352" windowHeight="7380"/>
   </bookViews>
   <sheets>
     <sheet name="TP" sheetId="1" r:id="rId1"/>
@@ -667,10 +667,10 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="3">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00\ _₫_-;\-* #,##0.00\ _₫_-;_-* &quot;-&quot;??\ _₫_-;_-@_-"/>
-    <numFmt numFmtId="165" formatCode="0.000"/>
-    <numFmt numFmtId="169" formatCode="_-* #,##0\ _₫_-;\-* #,##0\ _₫_-;_-* &quot;-&quot;??\ _₫_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="_-* #,##0\ _₫_-;\-* #,##0\ _₫_-;_-* &quot;-&quot;??\ _₫_-;_-@_-"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -695,6 +695,14 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -780,7 +788,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -798,12 +806,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -811,12 +813,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -835,39 +831,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -876,12 +845,52 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="169" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1189,8 +1198,8 @@
   </sheetPr>
   <dimension ref="A1:G57"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J42" sqref="J42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1201,36 +1210,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="34" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="34" t="s">
         <v>52</v>
       </c>
-      <c r="D1" s="24" t="s">
+      <c r="D1" s="30" t="s">
         <v>178</v>
       </c>
-      <c r="E1" s="34" t="s">
+      <c r="E1" s="32" t="s">
         <v>200</v>
       </c>
-      <c r="F1" s="24" t="s">
+      <c r="F1" s="30" t="s">
         <v>180</v>
       </c>
-      <c r="G1" s="36" t="s">
+      <c r="G1" s="29" t="s">
         <v>210</v>
       </c>
     </row>
     <row r="2" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="9"/>
-      <c r="B2" s="10"/>
-      <c r="C2" s="9"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="35"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="36"/>
+      <c r="A2" s="34"/>
+      <c r="B2" s="35"/>
+      <c r="C2" s="34"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="31"/>
+      <c r="G2" s="29"/>
     </row>
     <row r="3" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
@@ -1242,16 +1251,17 @@
       <c r="C3" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="D3" s="16" t="s">
-        <v>105</v>
-      </c>
-      <c r="E3" s="16">
+      <c r="D3" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="E3" s="12">
         <v>2</v>
       </c>
-      <c r="F3" s="16" t="s">
+      <c r="F3" s="12" t="s">
         <v>198</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="6">
+        <f>ROUNDUP(1/E3,0)</f>
         <v>1</v>
       </c>
     </row>
@@ -1265,17 +1275,17 @@
       <c r="C4" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D4" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="E4" s="11">
+      <c r="D4" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="E4" s="9">
         <v>1</v>
       </c>
-      <c r="F4" s="16" t="s">
+      <c r="F4" s="12" t="s">
         <v>198</v>
       </c>
       <c r="G4" s="6">
-        <f t="shared" ref="G4:G7" si="0">1/E4</f>
+        <f>ROUNDUP(1/E4,0)</f>
         <v>1</v>
       </c>
     </row>
@@ -1289,17 +1299,17 @@
       <c r="C5" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D5" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="E5" s="11">
+      <c r="D5" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="E5" s="9">
         <v>1</v>
       </c>
-      <c r="F5" s="16" t="s">
+      <c r="F5" s="12" t="s">
         <v>198</v>
       </c>
       <c r="G5" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="G5:G52" si="0">ROUNDUP(1/E5,0)</f>
         <v>1</v>
       </c>
     </row>
@@ -1313,13 +1323,13 @@
       <c r="C6" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D6" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="E6" s="11">
+      <c r="D6" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="E6" s="9">
         <v>1</v>
       </c>
-      <c r="F6" s="16" t="s">
+      <c r="F6" s="12" t="s">
         <v>198</v>
       </c>
       <c r="G6" s="6">
@@ -1337,13 +1347,13 @@
       <c r="C7" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="D7" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="E7" s="11">
+      <c r="D7" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="E7" s="9">
         <v>1</v>
       </c>
-      <c r="F7" s="16" t="s">
+      <c r="F7" s="12" t="s">
         <v>198</v>
       </c>
       <c r="G7" s="6">
@@ -1361,17 +1371,17 @@
       <c r="C8" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="D8" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="E8" s="11">
+      <c r="D8" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="E8" s="9">
         <v>0.5</v>
       </c>
-      <c r="F8" s="16" t="s">
+      <c r="F8" s="12" t="s">
         <v>198</v>
       </c>
       <c r="G8" s="6">
-        <f t="shared" ref="G8:G16" si="1">1/E8</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
     </row>
@@ -1385,17 +1395,17 @@
       <c r="C9" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="D9" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="E9" s="11">
+      <c r="D9" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="E9" s="9">
         <v>0.25</v>
       </c>
-      <c r="F9" s="16" t="s">
+      <c r="F9" s="12" t="s">
         <v>198</v>
       </c>
       <c r="G9" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
     </row>
@@ -1409,17 +1419,17 @@
       <c r="C10" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="D10" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="E10" s="11">
+      <c r="D10" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="E10" s="9">
         <v>0.2</v>
       </c>
-      <c r="F10" s="16" t="s">
+      <c r="F10" s="12" t="s">
         <v>198</v>
       </c>
       <c r="G10" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
     </row>
@@ -1433,17 +1443,17 @@
       <c r="C11" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="D11" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="E11" s="11">
+      <c r="D11" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="E11" s="9">
         <v>0.1</v>
       </c>
-      <c r="F11" s="16" t="s">
+      <c r="F11" s="12" t="s">
         <v>198</v>
       </c>
       <c r="G11" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
     </row>
@@ -1457,17 +1467,17 @@
       <c r="C12" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="D12" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="E12" s="11">
+      <c r="D12" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="E12" s="9">
         <v>0.02</v>
       </c>
-      <c r="F12" s="16" t="s">
+      <c r="F12" s="12" t="s">
         <v>198</v>
       </c>
       <c r="G12" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>50</v>
       </c>
     </row>
@@ -1481,17 +1491,17 @@
       <c r="C13" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="D13" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="E13" s="11">
+      <c r="D13" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="E13" s="9">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="F13" s="16" t="s">
+      <c r="F13" s="12" t="s">
         <v>198</v>
       </c>
       <c r="G13" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>40</v>
       </c>
     </row>
@@ -1505,17 +1515,17 @@
       <c r="C14" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="D14" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="E14" s="11">
+      <c r="D14" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="E14" s="9">
         <v>0.02</v>
       </c>
-      <c r="F14" s="16" t="s">
+      <c r="F14" s="12" t="s">
         <v>198</v>
       </c>
       <c r="G14" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>50</v>
       </c>
     </row>
@@ -1529,17 +1539,17 @@
       <c r="C15" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="D15" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="E15" s="11">
+      <c r="D15" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="E15" s="9">
         <v>0.01</v>
       </c>
-      <c r="F15" s="16" t="s">
+      <c r="F15" s="12" t="s">
         <v>198</v>
       </c>
       <c r="G15" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>100</v>
       </c>
     </row>
@@ -1553,17 +1563,17 @@
       <c r="C16" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="D16" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="E16" s="11">
+      <c r="D16" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="E16" s="9">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="F16" s="16" t="s">
+      <c r="F16" s="12" t="s">
         <v>198</v>
       </c>
       <c r="G16" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>200</v>
       </c>
     </row>
@@ -1577,17 +1587,17 @@
       <c r="C17" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="D17" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="E17" s="11">
+      <c r="D17" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="E17" s="9">
         <v>2E-3</v>
       </c>
-      <c r="F17" s="16" t="s">
+      <c r="F17" s="12" t="s">
         <v>198</v>
       </c>
       <c r="G17" s="6">
-        <f>1/E17</f>
+        <f t="shared" si="0"/>
         <v>500</v>
       </c>
     </row>
@@ -1601,12 +1611,18 @@
       <c r="C18" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D18" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="E18" s="11"/>
-      <c r="F18" s="11" t="s">
+      <c r="D18" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="E18" s="9">
+        <v>2</v>
+      </c>
+      <c r="F18" s="9" t="s">
         <v>199</v>
+      </c>
+      <c r="G18" s="6">
+        <f>ROUNDUP(1/E18,0)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
@@ -1619,12 +1635,18 @@
       <c r="C19" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="D19" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="E19" s="11"/>
-      <c r="F19" s="11" t="s">
+      <c r="D19" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="E19" s="9">
+        <v>1</v>
+      </c>
+      <c r="F19" s="9" t="s">
         <v>199</v>
+      </c>
+      <c r="G19" s="6">
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
@@ -1637,12 +1659,18 @@
       <c r="C20" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D20" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="E20" s="11"/>
-      <c r="F20" s="11" t="s">
+      <c r="D20" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="E20" s="9">
+        <v>1</v>
+      </c>
+      <c r="F20" s="9" t="s">
         <v>199</v>
+      </c>
+      <c r="G20" s="6">
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
@@ -1655,12 +1683,18 @@
       <c r="C21" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D21" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="E21" s="11"/>
-      <c r="F21" s="11" t="s">
+      <c r="D21" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="E21" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="F21" s="9" t="s">
         <v>199</v>
+      </c>
+      <c r="G21" s="6">
+        <f t="shared" si="0"/>
+        <v>2</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
@@ -1673,12 +1707,18 @@
       <c r="C22" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D22" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="E22" s="11"/>
-      <c r="F22" s="11" t="s">
+      <c r="D22" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="E22" s="9">
+        <v>0.2</v>
+      </c>
+      <c r="F22" s="9" t="s">
         <v>199</v>
+      </c>
+      <c r="G22" s="6">
+        <f t="shared" si="0"/>
+        <v>5</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
@@ -1691,12 +1731,18 @@
       <c r="C23" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="D23" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="E23" s="11"/>
-      <c r="F23" s="11" t="s">
+      <c r="D23" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="E23" s="9">
+        <v>0.1</v>
+      </c>
+      <c r="F23" s="9" t="s">
         <v>199</v>
+      </c>
+      <c r="G23" s="6">
+        <f t="shared" si="0"/>
+        <v>10</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
@@ -1709,12 +1755,18 @@
       <c r="C24" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D24" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="E24" s="11"/>
-      <c r="F24" s="11" t="s">
+      <c r="D24" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="E24" s="9">
+        <v>0.05</v>
+      </c>
+      <c r="F24" s="9" t="s">
         <v>199</v>
+      </c>
+      <c r="G24" s="6">
+        <f t="shared" si="0"/>
+        <v>20</v>
       </c>
     </row>
     <row r="25" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
@@ -1727,12 +1779,18 @@
       <c r="C25" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="D25" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="E25" s="11"/>
-      <c r="F25" s="11" t="s">
+      <c r="D25" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="E25" s="9">
+        <v>0.02</v>
+      </c>
+      <c r="F25" s="9" t="s">
         <v>199</v>
+      </c>
+      <c r="G25" s="6">
+        <f t="shared" si="0"/>
+        <v>50</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
@@ -1745,12 +1803,18 @@
       <c r="C26" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="D26" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="E26" s="11"/>
-      <c r="F26" s="11" t="s">
+      <c r="D26" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="E26" s="9">
+        <v>0.01</v>
+      </c>
+      <c r="F26" s="9" t="s">
         <v>199</v>
+      </c>
+      <c r="G26" s="6">
+        <f t="shared" si="0"/>
+        <v>100</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
@@ -1766,9 +1830,15 @@
       <c r="D27" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="E27" s="2"/>
-      <c r="F27" s="11" t="s">
+      <c r="E27" s="2">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="F27" s="9" t="s">
         <v>199</v>
+      </c>
+      <c r="G27" s="6">
+        <f t="shared" si="0"/>
+        <v>200</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
@@ -1784,9 +1854,15 @@
       <c r="D28" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="E28" s="2"/>
-      <c r="F28" s="11" t="s">
+      <c r="E28" s="2">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="F28" s="9" t="s">
         <v>199</v>
+      </c>
+      <c r="G28" s="6">
+        <f t="shared" si="0"/>
+        <v>334</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
@@ -1802,9 +1878,15 @@
       <c r="D29" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="E29" s="2"/>
-      <c r="F29" s="11" t="s">
+      <c r="E29" s="2">
+        <v>2E-3</v>
+      </c>
+      <c r="F29" s="9" t="s">
         <v>199</v>
+      </c>
+      <c r="G29" s="6">
+        <f t="shared" si="0"/>
+        <v>500</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
@@ -1820,9 +1902,15 @@
       <c r="D30" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="E30" s="2"/>
-      <c r="F30" s="11" t="s">
+      <c r="E30" s="2">
+        <v>1.4E-3</v>
+      </c>
+      <c r="F30" s="9" t="s">
         <v>199</v>
+      </c>
+      <c r="G30" s="6">
+        <f t="shared" si="0"/>
+        <v>715</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
@@ -1838,9 +1926,15 @@
       <c r="D31" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="E31" s="2"/>
-      <c r="F31" s="11" t="s">
+      <c r="E31" s="2">
+        <v>1</v>
+      </c>
+      <c r="F31" s="9" t="s">
         <v>199</v>
+      </c>
+      <c r="G31" s="6">
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
@@ -1856,12 +1950,18 @@
       <c r="D32" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="E32" s="2"/>
-      <c r="F32" s="11" t="s">
+      <c r="E32" s="2">
+        <v>1</v>
+      </c>
+      <c r="F32" s="9" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G32" s="6">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" s="2">
         <v>31</v>
       </c>
@@ -1874,12 +1974,18 @@
       <c r="D33" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="E33" s="2"/>
-      <c r="F33" s="11" t="s">
+      <c r="E33" s="2">
+        <v>1</v>
+      </c>
+      <c r="F33" s="9" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G33" s="6">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" s="2">
         <v>32</v>
       </c>
@@ -1892,12 +1998,18 @@
       <c r="D34" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="E34" s="2"/>
-      <c r="F34" s="11" t="s">
+      <c r="E34" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="F34" s="9" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G34" s="6">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" s="2">
         <v>33</v>
       </c>
@@ -1910,12 +2022,18 @@
       <c r="D35" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="E35" s="2"/>
-      <c r="F35" s="11" t="s">
+      <c r="E35" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="F35" s="9" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G35" s="6">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" s="2">
         <v>34</v>
       </c>
@@ -1928,12 +2046,18 @@
       <c r="D36" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="E36" s="2"/>
-      <c r="F36" s="11" t="s">
+      <c r="E36" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="F36" s="9" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G36" s="6">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" s="2">
         <v>35</v>
       </c>
@@ -1946,12 +2070,18 @@
       <c r="D37" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="E37" s="2"/>
-      <c r="F37" s="11" t="s">
+      <c r="E37" s="2">
+        <v>0.05</v>
+      </c>
+      <c r="F37" s="9" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G37" s="6">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" s="2">
         <v>36</v>
       </c>
@@ -1964,12 +2094,18 @@
       <c r="D38" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="E38" s="2"/>
-      <c r="F38" s="11" t="s">
+      <c r="E38" s="2">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="F38" s="9" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G38" s="6">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" s="2">
         <v>37</v>
       </c>
@@ -1982,12 +2118,18 @@
       <c r="D39" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="E39" s="2"/>
-      <c r="F39" s="11" t="s">
+      <c r="E39" s="2">
+        <v>0.02</v>
+      </c>
+      <c r="F39" s="9" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G39" s="6">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40" s="2">
         <v>38</v>
       </c>
@@ -2000,12 +2142,18 @@
       <c r="D40" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="E40" s="2"/>
-      <c r="F40" s="11" t="s">
+      <c r="E40" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="F40" s="9" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G40" s="6">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41" s="2">
         <v>39</v>
       </c>
@@ -2018,12 +2166,18 @@
       <c r="D41" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="E41" s="2"/>
-      <c r="F41" s="11" t="s">
+      <c r="E41" s="2">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="F41" s="9" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G41" s="6">
+        <f t="shared" si="0"/>
+        <v>200</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42" s="2">
         <v>40</v>
       </c>
@@ -2036,12 +2190,18 @@
       <c r="D42" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="E42" s="2"/>
-      <c r="F42" s="11" t="s">
+      <c r="E42" s="2">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="F42" s="9" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G42" s="6">
+        <f t="shared" si="0"/>
+        <v>334</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A43" s="2">
         <v>41</v>
       </c>
@@ -2054,12 +2214,18 @@
       <c r="D43" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="E43" s="2"/>
-      <c r="F43" s="11" t="s">
+      <c r="E43" s="2">
+        <v>2E-3</v>
+      </c>
+      <c r="F43" s="9" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G43" s="6">
+        <f t="shared" si="0"/>
+        <v>500</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A44" s="2">
         <v>42</v>
       </c>
@@ -2072,12 +2238,18 @@
       <c r="D44" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="E44" s="2"/>
-      <c r="F44" s="11" t="s">
+      <c r="E44" s="2">
+        <v>1.1999999999999999E-3</v>
+      </c>
+      <c r="F44" s="9" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="45" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G44" s="6">
+        <f t="shared" si="0"/>
+        <v>834</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="2">
         <v>43</v>
       </c>
@@ -2090,12 +2262,18 @@
       <c r="D45" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="E45" s="2"/>
+      <c r="E45" s="2">
+        <v>1E-3</v>
+      </c>
       <c r="F45" s="2" t="s">
         <v>198</v>
       </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G45" s="6">
+        <f t="shared" si="0"/>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A46" s="2">
         <v>44</v>
       </c>
@@ -2108,12 +2286,18 @@
       <c r="D46" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="E46" s="2"/>
+      <c r="E46" s="2">
+        <v>2E-3</v>
+      </c>
       <c r="F46" s="2" t="s">
         <v>198</v>
       </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G46" s="6">
+        <f t="shared" si="0"/>
+        <v>500</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A47" s="2">
         <v>45</v>
       </c>
@@ -2126,12 +2310,18 @@
       <c r="D47" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="E47" s="2"/>
+      <c r="E47" s="2">
+        <v>4.0000000000000001E-3</v>
+      </c>
       <c r="F47" s="2" t="s">
         <v>198</v>
       </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G47" s="6">
+        <f t="shared" si="0"/>
+        <v>250</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A48" s="2">
         <v>46</v>
       </c>
@@ -2144,12 +2334,18 @@
       <c r="D48" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="E48" s="2"/>
+      <c r="E48" s="2">
+        <v>8.0000000000000002E-3</v>
+      </c>
       <c r="F48" s="2" t="s">
         <v>198</v>
       </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G48" s="6">
+        <f t="shared" si="0"/>
+        <v>125</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A49" s="2">
         <v>47</v>
       </c>
@@ -2162,12 +2358,18 @@
       <c r="D49" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="E49" s="2"/>
+      <c r="E49" s="2">
+        <v>1.0999999999999999E-2</v>
+      </c>
       <c r="F49" s="2" t="s">
         <v>198</v>
       </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G49" s="6">
+        <f t="shared" si="0"/>
+        <v>91</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A50" s="2">
         <v>48</v>
       </c>
@@ -2180,12 +2382,18 @@
       <c r="D50" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="E50" s="2"/>
+      <c r="E50" s="2">
+        <v>1.7000000000000001E-2</v>
+      </c>
       <c r="F50" s="2" t="s">
         <v>198</v>
       </c>
-    </row>
-    <row r="51" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G50" s="6">
+        <f t="shared" si="0"/>
+        <v>59</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="2">
         <v>49</v>
       </c>
@@ -2198,12 +2406,18 @@
       <c r="D51" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="E51" s="2"/>
+      <c r="E51" s="2">
+        <v>5.0000000000000001E-3</v>
+      </c>
       <c r="F51" s="2" t="s">
         <v>198</v>
       </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G51" s="6">
+        <f t="shared" si="0"/>
+        <v>200</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A52" s="2">
         <v>50</v>
       </c>
@@ -2216,12 +2430,18 @@
       <c r="D52" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="E52" s="2"/>
+      <c r="E52" s="2">
+        <v>0.01</v>
+      </c>
       <c r="F52" s="2" t="s">
         <v>198</v>
       </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G52" s="6">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A57" s="8"/>
     </row>
   </sheetData>
@@ -2258,55 +2478,55 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="36" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="37" t="s">
         <v>103</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="36" t="s">
         <v>52</v>
       </c>
-      <c r="D1" s="24" t="s">
+      <c r="D1" s="30" t="s">
         <v>178</v>
       </c>
-      <c r="E1" s="24" t="s">
+      <c r="E1" s="30" t="s">
         <v>179</v>
       </c>
-      <c r="F1" s="24" t="s">
+      <c r="F1" s="30" t="s">
         <v>180</v>
       </c>
-      <c r="G1" s="24" t="s">
+      <c r="G1" s="30" t="s">
         <v>181</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="14"/>
-      <c r="B2" s="15"/>
-      <c r="C2" s="14"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="25"/>
+      <c r="A2" s="36"/>
+      <c r="B2" s="37"/>
+      <c r="C2" s="36"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="31"/>
+      <c r="G2" s="31"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="4">
         <v>1</v>
       </c>
       <c r="B3" s="5"/>
-      <c r="C3" s="16" t="s">
+      <c r="C3" s="12" t="s">
         <v>104</v>
       </c>
-      <c r="D3" s="16" t="s">
-        <v>105</v>
-      </c>
-      <c r="E3" s="16" t="s">
+      <c r="D3" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="E3" s="12" t="s">
         <v>106</v>
       </c>
-      <c r="F3" s="16" t="s">
-        <v>107</v>
-      </c>
-      <c r="G3" s="17" t="s">
+      <c r="F3" s="12" t="s">
+        <v>107</v>
+      </c>
+      <c r="G3" s="13" t="s">
         <v>108</v>
       </c>
     </row>
@@ -2315,19 +2535,19 @@
         <v>2</v>
       </c>
       <c r="B4" s="5"/>
-      <c r="C4" s="11" t="s">
+      <c r="C4" s="9" t="s">
         <v>109</v>
       </c>
-      <c r="D4" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="E4" s="11" t="s">
+      <c r="D4" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="E4" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="F4" s="11" t="s">
-        <v>107</v>
-      </c>
-      <c r="G4" s="18" t="s">
+      <c r="F4" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="G4" s="14" t="s">
         <v>111</v>
       </c>
     </row>
@@ -2336,19 +2556,19 @@
         <v>3</v>
       </c>
       <c r="B5" s="5"/>
-      <c r="C5" s="11" t="s">
+      <c r="C5" s="9" t="s">
         <v>112</v>
       </c>
-      <c r="D5" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="E5" s="19" t="s">
+      <c r="D5" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="E5" s="15" t="s">
         <v>113</v>
       </c>
-      <c r="F5" s="11" t="s">
-        <v>107</v>
-      </c>
-      <c r="G5" s="18" t="s">
+      <c r="F5" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="G5" s="14" t="s">
         <v>114</v>
       </c>
     </row>
@@ -2357,19 +2577,19 @@
         <v>4</v>
       </c>
       <c r="B6" s="5"/>
-      <c r="C6" s="11" t="s">
+      <c r="C6" s="9" t="s">
         <v>115</v>
       </c>
-      <c r="D6" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="E6" s="11" t="s">
+      <c r="D6" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="E6" s="9" t="s">
         <v>116</v>
       </c>
-      <c r="F6" s="11" t="s">
-        <v>107</v>
-      </c>
-      <c r="G6" s="18" t="s">
+      <c r="F6" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="G6" s="14" t="s">
         <v>117</v>
       </c>
     </row>
@@ -2378,19 +2598,19 @@
         <v>5</v>
       </c>
       <c r="B7" s="5"/>
-      <c r="C7" s="11" t="s">
+      <c r="C7" s="9" t="s">
         <v>118</v>
       </c>
-      <c r="D7" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="E7" s="11" t="s">
+      <c r="D7" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="E7" s="9" t="s">
         <v>119</v>
       </c>
-      <c r="F7" s="11" t="s">
-        <v>107</v>
-      </c>
-      <c r="G7" s="12" t="s">
+      <c r="F7" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="G7" s="10" t="s">
         <v>120</v>
       </c>
     </row>
@@ -2399,19 +2619,19 @@
         <v>6</v>
       </c>
       <c r="B8" s="5"/>
-      <c r="C8" s="11" t="s">
+      <c r="C8" s="9" t="s">
         <v>121</v>
       </c>
-      <c r="D8" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="E8" s="11" t="s">
+      <c r="D8" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="E8" s="9" t="s">
         <v>122</v>
       </c>
-      <c r="F8" s="11" t="s">
-        <v>107</v>
-      </c>
-      <c r="G8" s="12" t="s">
+      <c r="F8" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="G8" s="10" t="s">
         <v>123</v>
       </c>
     </row>
@@ -2420,19 +2640,19 @@
         <v>7</v>
       </c>
       <c r="B9" s="5"/>
-      <c r="C9" s="11" t="s">
+      <c r="C9" s="9" t="s">
         <v>124</v>
       </c>
-      <c r="D9" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="E9" s="11" t="s">
+      <c r="D9" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="E9" s="9" t="s">
         <v>125</v>
       </c>
-      <c r="F9" s="11" t="s">
-        <v>107</v>
-      </c>
-      <c r="G9" s="12" t="s">
+      <c r="F9" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="G9" s="10" t="s">
         <v>126</v>
       </c>
     </row>
@@ -2441,19 +2661,19 @@
         <v>8</v>
       </c>
       <c r="B10" s="5"/>
-      <c r="C10" s="11" t="s">
+      <c r="C10" s="9" t="s">
         <v>127</v>
       </c>
-      <c r="D10" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="E10" s="11" t="s">
+      <c r="D10" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="E10" s="9" t="s">
         <v>128</v>
       </c>
-      <c r="F10" s="11" t="s">
-        <v>107</v>
-      </c>
-      <c r="G10" s="12" t="s">
+      <c r="F10" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="G10" s="10" t="s">
         <v>129</v>
       </c>
     </row>
@@ -2462,19 +2682,19 @@
         <v>9</v>
       </c>
       <c r="B11" s="5"/>
-      <c r="C11" s="11" t="s">
+      <c r="C11" s="9" t="s">
         <v>130</v>
       </c>
-      <c r="D11" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="E11" s="11" t="s">
+      <c r="D11" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="E11" s="9" t="s">
         <v>131</v>
       </c>
-      <c r="F11" s="11" t="s">
-        <v>107</v>
-      </c>
-      <c r="G11" s="12" t="s">
+      <c r="F11" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="G11" s="10" t="s">
         <v>132</v>
       </c>
     </row>
@@ -2483,19 +2703,19 @@
         <v>10</v>
       </c>
       <c r="B12" s="5"/>
-      <c r="C12" s="11" t="s">
+      <c r="C12" s="9" t="s">
         <v>133</v>
       </c>
-      <c r="D12" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="E12" s="11" t="s">
+      <c r="D12" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="E12" s="9" t="s">
         <v>134</v>
       </c>
-      <c r="F12" s="11" t="s">
-        <v>107</v>
-      </c>
-      <c r="G12" s="18" t="s">
+      <c r="F12" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="G12" s="14" t="s">
         <v>135</v>
       </c>
     </row>
@@ -2504,19 +2724,19 @@
         <v>11</v>
       </c>
       <c r="B13" s="5"/>
-      <c r="C13" s="11" t="s">
+      <c r="C13" s="9" t="s">
         <v>136</v>
       </c>
-      <c r="D13" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="E13" s="11" t="s">
+      <c r="D13" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="E13" s="9" t="s">
         <v>137</v>
       </c>
-      <c r="F13" s="11" t="s">
-        <v>107</v>
-      </c>
-      <c r="G13" s="12" t="s">
+      <c r="F13" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="G13" s="10" t="s">
         <v>138</v>
       </c>
     </row>
@@ -2525,19 +2745,19 @@
         <v>12</v>
       </c>
       <c r="B14" s="5"/>
-      <c r="C14" s="11" t="s">
+      <c r="C14" s="9" t="s">
         <v>139</v>
       </c>
-      <c r="D14" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="E14" s="11" t="s">
+      <c r="D14" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="E14" s="9" t="s">
         <v>140</v>
       </c>
-      <c r="F14" s="11" t="s">
-        <v>107</v>
-      </c>
-      <c r="G14" s="12" t="s">
+      <c r="F14" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="G14" s="10" t="s">
         <v>141</v>
       </c>
     </row>
@@ -2546,19 +2766,19 @@
         <v>13</v>
       </c>
       <c r="B15" s="5"/>
-      <c r="C15" s="11" t="s">
+      <c r="C15" s="9" t="s">
         <v>142</v>
       </c>
-      <c r="D15" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="E15" s="11" t="s">
+      <c r="D15" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="E15" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="F15" s="11" t="s">
-        <v>107</v>
-      </c>
-      <c r="G15" s="11" t="s">
+      <c r="F15" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="G15" s="9" t="s">
         <v>144</v>
       </c>
     </row>
@@ -2567,19 +2787,19 @@
         <v>14</v>
       </c>
       <c r="B16" s="5"/>
-      <c r="C16" s="11" t="s">
+      <c r="C16" s="9" t="s">
         <v>145</v>
       </c>
-      <c r="D16" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="E16" s="11" t="s">
+      <c r="D16" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="E16" s="9" t="s">
         <v>146</v>
       </c>
-      <c r="F16" s="11" t="s">
-        <v>107</v>
-      </c>
-      <c r="G16" s="11" t="s">
+      <c r="F16" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="G16" s="9" t="s">
         <v>147</v>
       </c>
     </row>
@@ -2588,19 +2808,19 @@
         <v>15</v>
       </c>
       <c r="B17" s="5"/>
-      <c r="C17" s="11" t="s">
+      <c r="C17" s="9" t="s">
         <v>148</v>
       </c>
-      <c r="D17" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="E17" s="11" t="s">
+      <c r="D17" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="E17" s="9" t="s">
         <v>149</v>
       </c>
-      <c r="F17" s="11" t="s">
-        <v>107</v>
-      </c>
-      <c r="G17" s="11" t="s">
+      <c r="F17" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="G17" s="9" t="s">
         <v>150</v>
       </c>
     </row>
@@ -2609,19 +2829,19 @@
         <v>16</v>
       </c>
       <c r="B18" s="5"/>
-      <c r="C18" s="11" t="s">
+      <c r="C18" s="9" t="s">
         <v>151</v>
       </c>
-      <c r="D18" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="E18" s="11" t="s">
+      <c r="D18" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="E18" s="9" t="s">
         <v>152</v>
       </c>
-      <c r="F18" s="11" t="s">
-        <v>107</v>
-      </c>
-      <c r="G18" s="11" t="s">
+      <c r="F18" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="G18" s="9" t="s">
         <v>153</v>
       </c>
     </row>
@@ -2630,19 +2850,19 @@
         <v>17</v>
       </c>
       <c r="B19" s="5"/>
-      <c r="C19" s="11" t="s">
+      <c r="C19" s="9" t="s">
         <v>154</v>
       </c>
-      <c r="D19" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="E19" s="11" t="s">
+      <c r="D19" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="E19" s="9" t="s">
         <v>155</v>
       </c>
-      <c r="F19" s="11" t="s">
-        <v>107</v>
-      </c>
-      <c r="G19" s="11" t="s">
+      <c r="F19" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="G19" s="9" t="s">
         <v>156</v>
       </c>
     </row>
@@ -2651,19 +2871,19 @@
         <v>18</v>
       </c>
       <c r="B20" s="5"/>
-      <c r="C20" s="11" t="s">
+      <c r="C20" s="9" t="s">
         <v>157</v>
       </c>
-      <c r="D20" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="E20" s="11" t="s">
+      <c r="D20" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="E20" s="9" t="s">
         <v>158</v>
       </c>
-      <c r="F20" s="11" t="s">
-        <v>107</v>
-      </c>
-      <c r="G20" s="11" t="s">
+      <c r="F20" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="G20" s="9" t="s">
         <v>159</v>
       </c>
     </row>
@@ -2672,19 +2892,19 @@
         <v>19</v>
       </c>
       <c r="B21" s="5"/>
-      <c r="C21" s="11" t="s">
+      <c r="C21" s="9" t="s">
         <v>160</v>
       </c>
-      <c r="D21" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="E21" s="11" t="s">
+      <c r="D21" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="E21" s="9" t="s">
         <v>161</v>
       </c>
-      <c r="F21" s="11" t="s">
-        <v>107</v>
-      </c>
-      <c r="G21" s="11" t="s">
+      <c r="F21" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="G21" s="9" t="s">
         <v>162</v>
       </c>
     </row>
@@ -2693,19 +2913,19 @@
         <v>20</v>
       </c>
       <c r="B22" s="5"/>
-      <c r="C22" s="11" t="s">
+      <c r="C22" s="9" t="s">
         <v>163</v>
       </c>
-      <c r="D22" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="E22" s="11" t="s">
+      <c r="D22" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="E22" s="9" t="s">
         <v>164</v>
       </c>
-      <c r="F22" s="11" t="s">
-        <v>107</v>
-      </c>
-      <c r="G22" s="11" t="s">
+      <c r="F22" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="G22" s="9" t="s">
         <v>165</v>
       </c>
     </row>
@@ -2714,19 +2934,19 @@
         <v>21</v>
       </c>
       <c r="B23" s="5"/>
-      <c r="C23" s="11" t="s">
+      <c r="C23" s="9" t="s">
         <v>166</v>
       </c>
-      <c r="D23" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="E23" s="11" t="s">
+      <c r="D23" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="E23" s="9" t="s">
         <v>167</v>
       </c>
-      <c r="F23" s="11" t="s">
-        <v>107</v>
-      </c>
-      <c r="G23" s="11" t="s">
+      <c r="F23" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="G23" s="9" t="s">
         <v>168</v>
       </c>
     </row>
@@ -2735,19 +2955,19 @@
         <v>22</v>
       </c>
       <c r="B24" s="5"/>
-      <c r="C24" s="11" t="s">
+      <c r="C24" s="9" t="s">
         <v>169</v>
       </c>
-      <c r="D24" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="E24" s="11" t="s">
+      <c r="D24" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="E24" s="9" t="s">
         <v>170</v>
       </c>
-      <c r="F24" s="11" t="s">
-        <v>107</v>
-      </c>
-      <c r="G24" s="11" t="s">
+      <c r="F24" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="G24" s="9" t="s">
         <v>171</v>
       </c>
     </row>
@@ -2756,19 +2976,19 @@
         <v>23</v>
       </c>
       <c r="B25" s="5"/>
-      <c r="C25" s="11" t="s">
+      <c r="C25" s="9" t="s">
         <v>172</v>
       </c>
-      <c r="D25" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="E25" s="11" t="s">
+      <c r="D25" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="E25" s="9" t="s">
         <v>173</v>
       </c>
-      <c r="F25" s="11" t="s">
-        <v>107</v>
-      </c>
-      <c r="G25" s="11" t="s">
+      <c r="F25" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="G25" s="9" t="s">
         <v>174</v>
       </c>
     </row>
@@ -2777,19 +2997,19 @@
         <v>24</v>
       </c>
       <c r="B26" s="5"/>
-      <c r="C26" s="11" t="s">
+      <c r="C26" s="9" t="s">
         <v>175</v>
       </c>
-      <c r="D26" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="E26" s="11" t="s">
+      <c r="D26" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="E26" s="9" t="s">
         <v>176</v>
       </c>
-      <c r="F26" s="11" t="s">
-        <v>107</v>
-      </c>
-      <c r="G26" s="11" t="s">
+      <c r="F26" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="G26" s="9" t="s">
         <v>177</v>
       </c>
     </row>
@@ -2810,7 +3030,7 @@
       <c r="F27" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="G27" s="20" t="s">
+      <c r="G27" s="16" t="s">
         <v>184</v>
       </c>
     </row>
@@ -2831,7 +3051,7 @@
       <c r="F28" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="G28" s="20" t="s">
+      <c r="G28" s="16" t="s">
         <v>186</v>
       </c>
     </row>
@@ -2846,13 +3066,13 @@
       <c r="D29" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="E29" s="21" t="s">
+      <c r="E29" s="17" t="s">
         <v>188</v>
       </c>
       <c r="F29" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="G29" s="20" t="s">
+      <c r="G29" s="16" t="s">
         <v>189</v>
       </c>
     </row>
@@ -2867,13 +3087,13 @@
       <c r="D30" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="E30" s="21" t="s">
+      <c r="E30" s="17" t="s">
         <v>193</v>
       </c>
       <c r="F30" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="G30" s="20" t="s">
+      <c r="G30" s="16" t="s">
         <v>192</v>
       </c>
     </row>
@@ -2888,13 +3108,13 @@
       <c r="D31" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="E31" s="21" t="s">
+      <c r="E31" s="17" t="s">
         <v>196</v>
       </c>
-      <c r="F31" s="22" t="s">
+      <c r="F31" s="18" t="s">
         <v>195</v>
       </c>
-      <c r="G31" s="23" t="s">
+      <c r="G31" s="19" t="s">
         <v>197</v>
       </c>
     </row>
@@ -3151,8 +3371,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3160,49 +3380,49 @@
     <col min="1" max="1" width="3.44140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.44140625" style="7" customWidth="1"/>
     <col min="3" max="3" width="28.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.33203125" style="33" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.33203125" style="23" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8" customWidth="1"/>
     <col min="6" max="6" width="11.88671875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="34" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="34" t="s">
         <v>52</v>
       </c>
-      <c r="D1" s="28" t="s">
+      <c r="D1" s="39" t="s">
         <v>204</v>
       </c>
-      <c r="E1" s="26" t="s">
+      <c r="E1" s="41" t="s">
         <v>211</v>
       </c>
-      <c r="F1" s="26" t="s">
+      <c r="F1" s="41" t="s">
         <v>212</v>
       </c>
-      <c r="G1" s="42"/>
-      <c r="H1" s="13"/>
-      <c r="I1" s="13"/>
-      <c r="J1" s="13"/>
-      <c r="K1" s="13"/>
+      <c r="G1" s="38"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="11"/>
+      <c r="K1" s="11"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A2" s="9"/>
-      <c r="B2" s="10"/>
-      <c r="C2" s="9"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27"/>
-      <c r="G2" s="42"/>
-      <c r="H2" s="13"/>
-      <c r="I2" s="13"/>
-      <c r="J2" s="13"/>
-      <c r="K2" s="13"/>
+      <c r="A2" s="34"/>
+      <c r="B2" s="35"/>
+      <c r="C2" s="34"/>
+      <c r="D2" s="40"/>
+      <c r="E2" s="42"/>
+      <c r="F2" s="42"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
+      <c r="J2" s="11"/>
+      <c r="K2" s="11"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
@@ -3212,13 +3432,13 @@
       <c r="C3" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="D3" s="37">
+      <c r="D3" s="24">
         <v>0.5</v>
       </c>
-      <c r="E3" s="30" t="s">
-        <v>107</v>
-      </c>
-      <c r="F3" s="41">
+      <c r="E3" s="20" t="s">
+        <v>107</v>
+      </c>
+      <c r="F3" s="28">
         <v>12000</v>
       </c>
       <c r="G3">
@@ -3234,18 +3454,18 @@
       <c r="C4" s="2" t="s">
         <v>202</v>
       </c>
-      <c r="D4" s="37">
-        <v>0.2</v>
-      </c>
-      <c r="E4" s="30" t="s">
-        <v>107</v>
-      </c>
-      <c r="F4" s="41">
-        <v>13500</v>
+      <c r="D4" s="24">
+        <v>0.25</v>
+      </c>
+      <c r="E4" s="20" t="s">
+        <v>107</v>
+      </c>
+      <c r="F4" s="28">
+        <v>9000</v>
       </c>
       <c r="G4">
         <f t="shared" ref="G4:G8" si="0">F4*D4</f>
-        <v>2700</v>
+        <v>2250</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
@@ -3256,18 +3476,18 @@
       <c r="C5" s="2" t="s">
         <v>203</v>
       </c>
-      <c r="D5" s="37">
-        <v>0.25</v>
-      </c>
-      <c r="E5" s="30" t="s">
-        <v>107</v>
-      </c>
-      <c r="F5" s="41">
+      <c r="D5" s="24">
+        <v>0.2</v>
+      </c>
+      <c r="E5" s="20" t="s">
+        <v>107</v>
+      </c>
+      <c r="F5" s="28">
         <v>3000</v>
       </c>
       <c r="G5">
         <f t="shared" si="0"/>
-        <v>750</v>
+        <v>600</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
@@ -3275,21 +3495,19 @@
         <v>4</v>
       </c>
       <c r="B6" s="3"/>
-      <c r="C6" s="11" t="s">
+      <c r="C6" s="9" t="s">
         <v>118</v>
       </c>
-      <c r="D6" s="37">
-        <v>0.02</v>
-      </c>
-      <c r="E6" s="30" t="s">
-        <v>107</v>
-      </c>
-      <c r="F6" s="41">
+      <c r="D6" s="24"/>
+      <c r="E6" s="20" t="s">
+        <v>107</v>
+      </c>
+      <c r="F6" s="28">
         <v>80000</v>
       </c>
       <c r="G6">
         <f t="shared" si="0"/>
-        <v>1600</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
@@ -3297,21 +3515,19 @@
         <v>5</v>
       </c>
       <c r="B7" s="3"/>
-      <c r="C7" s="11" t="s">
+      <c r="C7" s="9" t="s">
         <v>121</v>
       </c>
-      <c r="D7" s="37">
-        <v>0.01</v>
-      </c>
-      <c r="E7" s="30" t="s">
-        <v>107</v>
-      </c>
-      <c r="F7" s="41">
+      <c r="D7" s="24"/>
+      <c r="E7" s="20" t="s">
+        <v>107</v>
+      </c>
+      <c r="F7" s="28">
         <v>80000</v>
       </c>
       <c r="G7">
         <f t="shared" si="0"/>
-        <v>800</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
@@ -3319,21 +3535,21 @@
         <v>6</v>
       </c>
       <c r="B8" s="3"/>
-      <c r="C8" s="11" t="s">
+      <c r="C8" s="9" t="s">
         <v>109</v>
       </c>
-      <c r="D8" s="37">
-        <v>0.02</v>
-      </c>
-      <c r="E8" s="30" t="s">
-        <v>107</v>
-      </c>
-      <c r="F8" s="41">
+      <c r="D8" s="24">
+        <v>0.05</v>
+      </c>
+      <c r="E8" s="20" t="s">
+        <v>107</v>
+      </c>
+      <c r="F8" s="28">
         <v>130000</v>
       </c>
       <c r="G8">
         <f t="shared" si="0"/>
-        <v>2600</v>
+        <v>6500</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
@@ -3342,13 +3558,13 @@
       <c r="C9" s="4" t="s">
         <v>207</v>
       </c>
-      <c r="D9" s="38">
+      <c r="D9" s="25">
         <v>0.6</v>
       </c>
-      <c r="E9" s="30" t="s">
+      <c r="E9" s="20" t="s">
         <v>206</v>
       </c>
-      <c r="F9" s="41"/>
+      <c r="F9" s="28"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="2"/>
@@ -3356,13 +3572,13 @@
       <c r="C10" s="4" t="s">
         <v>208</v>
       </c>
-      <c r="D10" s="38">
+      <c r="D10" s="25">
         <v>0.2</v>
       </c>
-      <c r="E10" s="30" t="s">
+      <c r="E10" s="20" t="s">
         <v>206</v>
       </c>
-      <c r="F10" s="41"/>
+      <c r="F10" s="28"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="2"/>
@@ -3370,13 +3586,13 @@
       <c r="C11" s="2" t="s">
         <v>203</v>
       </c>
-      <c r="D11" s="37">
+      <c r="D11" s="24">
         <v>0.2</v>
       </c>
-      <c r="E11" s="30" t="s">
+      <c r="E11" s="20" t="s">
         <v>206</v>
       </c>
-      <c r="F11" s="41"/>
+      <c r="F11" s="28"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" s="2"/>
@@ -3384,13 +3600,13 @@
       <c r="C12" s="4" t="s">
         <v>182</v>
       </c>
-      <c r="D12" s="37">
+      <c r="D12" s="24">
         <v>0.1</v>
       </c>
-      <c r="E12" s="30" t="s">
+      <c r="E12" s="20" t="s">
         <v>205</v>
       </c>
-      <c r="F12" s="41"/>
+      <c r="F12" s="28"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="2"/>
@@ -3398,13 +3614,13 @@
       <c r="C13" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="D13" s="37">
+      <c r="D13" s="24">
         <v>0.89</v>
       </c>
-      <c r="E13" s="30" t="s">
+      <c r="E13" s="20" t="s">
         <v>205</v>
       </c>
-      <c r="F13" s="41"/>
+      <c r="F13" s="28"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="2"/>
@@ -3412,265 +3628,269 @@
       <c r="C14" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="D14" s="37">
+      <c r="D14" s="24">
         <v>2E-3</v>
       </c>
-      <c r="E14" s="30" t="s">
+      <c r="E14" s="20" t="s">
         <v>205</v>
       </c>
-      <c r="F14" s="41"/>
+      <c r="F14" s="28"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" s="2"/>
       <c r="B15" s="3"/>
-      <c r="C15" s="11" t="s">
+      <c r="C15" s="9" t="s">
         <v>118</v>
       </c>
-      <c r="D15" s="37">
+      <c r="D15" s="24">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="E15" s="30" t="s">
+      <c r="E15" s="20" t="s">
         <v>205</v>
       </c>
-      <c r="F15" s="41"/>
+      <c r="F15" s="28"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" s="2"/>
       <c r="B16" s="3"/>
       <c r="C16" s="2"/>
-      <c r="D16" s="31"/>
-      <c r="E16" s="30"/>
-      <c r="F16" s="41"/>
+      <c r="D16" s="21"/>
+      <c r="E16" s="20"/>
+      <c r="F16" s="28"/>
+      <c r="G16" s="43">
+        <f>SUM(G3:G8)</f>
+        <v>15350</v>
+      </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="2"/>
       <c r="B17" s="5"/>
       <c r="C17" s="4"/>
-      <c r="D17" s="32"/>
-      <c r="E17" s="30"/>
-      <c r="F17" s="39"/>
+      <c r="D17" s="22"/>
+      <c r="E17" s="20"/>
+      <c r="F17" s="26"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="2"/>
       <c r="B18" s="3"/>
       <c r="C18" s="2"/>
-      <c r="D18" s="31"/>
-      <c r="E18" s="11"/>
-      <c r="F18" s="40"/>
+      <c r="D18" s="21"/>
+      <c r="E18" s="9"/>
+      <c r="F18" s="27"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="2"/>
       <c r="B19" s="3"/>
       <c r="C19" s="2"/>
-      <c r="D19" s="31"/>
-      <c r="E19" s="11"/>
-      <c r="F19" s="40"/>
+      <c r="D19" s="21"/>
+      <c r="E19" s="9"/>
+      <c r="F19" s="27"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="2"/>
       <c r="B20" s="3"/>
       <c r="C20" s="2"/>
-      <c r="D20" s="31"/>
-      <c r="E20" s="11"/>
-      <c r="F20" s="40"/>
+      <c r="D20" s="21"/>
+      <c r="E20" s="9"/>
+      <c r="F20" s="27"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="2"/>
       <c r="B21" s="3"/>
       <c r="C21" s="2"/>
-      <c r="D21" s="31"/>
-      <c r="E21" s="11"/>
-      <c r="F21" s="40"/>
+      <c r="D21" s="21"/>
+      <c r="E21" s="9"/>
+      <c r="F21" s="27"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="2"/>
       <c r="B22" s="3"/>
       <c r="C22" s="2"/>
-      <c r="D22" s="31"/>
-      <c r="E22" s="11"/>
-      <c r="F22" s="40"/>
+      <c r="D22" s="21"/>
+      <c r="E22" s="9"/>
+      <c r="F22" s="27"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="2"/>
       <c r="B23" s="3"/>
       <c r="C23" s="2"/>
-      <c r="D23" s="31"/>
-      <c r="E23" s="11"/>
-      <c r="F23" s="40"/>
+      <c r="D23" s="21"/>
+      <c r="E23" s="9"/>
+      <c r="F23" s="27"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="2"/>
       <c r="B24" s="3"/>
       <c r="C24" s="2"/>
-      <c r="D24" s="31"/>
-      <c r="E24" s="11"/>
-      <c r="F24" s="11"/>
+      <c r="D24" s="21"/>
+      <c r="E24" s="9"/>
+      <c r="F24" s="9"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="2"/>
       <c r="B25" s="3"/>
       <c r="C25" s="4"/>
-      <c r="D25" s="32"/>
-      <c r="E25" s="11"/>
-      <c r="F25" s="11"/>
+      <c r="D25" s="22"/>
+      <c r="E25" s="9"/>
+      <c r="F25" s="9"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" s="2"/>
       <c r="B26" s="3"/>
       <c r="C26" s="2"/>
-      <c r="D26" s="31"/>
-      <c r="E26" s="11"/>
-      <c r="F26" s="11"/>
+      <c r="D26" s="21"/>
+      <c r="E26" s="9"/>
+      <c r="F26" s="9"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" s="2"/>
       <c r="B27" s="3"/>
       <c r="C27" s="2"/>
-      <c r="D27" s="31"/>
+      <c r="D27" s="21"/>
       <c r="E27" s="2"/>
-      <c r="F27" s="11"/>
+      <c r="F27" s="9"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" s="2"/>
       <c r="B28" s="3"/>
       <c r="C28" s="2"/>
-      <c r="D28" s="31"/>
+      <c r="D28" s="21"/>
       <c r="E28" s="2"/>
-      <c r="F28" s="11"/>
+      <c r="F28" s="9"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" s="2"/>
       <c r="B29" s="3"/>
       <c r="C29" s="2"/>
-      <c r="D29" s="31"/>
+      <c r="D29" s="21"/>
       <c r="E29" s="2"/>
-      <c r="F29" s="11"/>
+      <c r="F29" s="9"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" s="2"/>
       <c r="B30" s="3"/>
       <c r="C30" s="2"/>
-      <c r="D30" s="31"/>
+      <c r="D30" s="21"/>
       <c r="E30" s="2"/>
-      <c r="F30" s="11"/>
+      <c r="F30" s="9"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" s="2"/>
       <c r="B31" s="3"/>
       <c r="C31" s="4"/>
-      <c r="D31" s="32"/>
+      <c r="D31" s="22"/>
       <c r="E31" s="2"/>
-      <c r="F31" s="11"/>
+      <c r="F31" s="9"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" s="2"/>
       <c r="B32" s="3"/>
       <c r="C32" s="4"/>
-      <c r="D32" s="32"/>
+      <c r="D32" s="22"/>
       <c r="E32" s="2"/>
-      <c r="F32" s="11"/>
+      <c r="F32" s="9"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" s="2"/>
       <c r="B33" s="3"/>
       <c r="C33" s="4"/>
-      <c r="D33" s="32"/>
+      <c r="D33" s="22"/>
       <c r="E33" s="2"/>
-      <c r="F33" s="11"/>
+      <c r="F33" s="9"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" s="2"/>
       <c r="B34" s="3"/>
       <c r="C34" s="4"/>
-      <c r="D34" s="32"/>
+      <c r="D34" s="22"/>
       <c r="E34" s="2"/>
-      <c r="F34" s="11"/>
+      <c r="F34" s="9"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" s="2"/>
       <c r="B35" s="3"/>
       <c r="C35" s="4"/>
-      <c r="D35" s="32"/>
+      <c r="D35" s="22"/>
       <c r="E35" s="2"/>
-      <c r="F35" s="11"/>
+      <c r="F35" s="9"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" s="2"/>
       <c r="B36" s="3"/>
       <c r="C36" s="4"/>
-      <c r="D36" s="32"/>
+      <c r="D36" s="22"/>
       <c r="E36" s="2"/>
-      <c r="F36" s="11"/>
+      <c r="F36" s="9"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" s="2"/>
       <c r="B37" s="3"/>
       <c r="C37" s="4"/>
-      <c r="D37" s="32"/>
+      <c r="D37" s="22"/>
       <c r="E37" s="2"/>
-      <c r="F37" s="11"/>
+      <c r="F37" s="9"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" s="2"/>
       <c r="B38" s="3"/>
       <c r="C38" s="4"/>
-      <c r="D38" s="32"/>
+      <c r="D38" s="22"/>
       <c r="E38" s="2"/>
-      <c r="F38" s="11"/>
+      <c r="F38" s="9"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" s="2"/>
       <c r="B39" s="3"/>
       <c r="C39" s="4"/>
-      <c r="D39" s="32"/>
+      <c r="D39" s="22"/>
       <c r="E39" s="2"/>
-      <c r="F39" s="11"/>
+      <c r="F39" s="9"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" s="2"/>
       <c r="B40" s="3"/>
       <c r="C40" s="4"/>
-      <c r="D40" s="32"/>
+      <c r="D40" s="22"/>
       <c r="E40" s="2"/>
-      <c r="F40" s="11"/>
+      <c r="F40" s="9"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" s="2"/>
       <c r="B41" s="3"/>
       <c r="C41" s="4"/>
-      <c r="D41" s="32"/>
+      <c r="D41" s="22"/>
       <c r="E41" s="2"/>
-      <c r="F41" s="11"/>
+      <c r="F41" s="9"/>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" s="2"/>
       <c r="B42" s="3"/>
       <c r="C42" s="4"/>
-      <c r="D42" s="32"/>
+      <c r="D42" s="22"/>
       <c r="E42" s="2"/>
-      <c r="F42" s="11"/>
+      <c r="F42" s="9"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" s="2"/>
       <c r="B43" s="3"/>
       <c r="C43" s="4"/>
-      <c r="D43" s="32"/>
+      <c r="D43" s="22"/>
       <c r="E43" s="2"/>
-      <c r="F43" s="11"/>
+      <c r="F43" s="9"/>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" s="2"/>
       <c r="B44" s="3"/>
       <c r="C44" s="4"/>
-      <c r="D44" s="32"/>
+      <c r="D44" s="22"/>
       <c r="E44" s="2"/>
-      <c r="F44" s="11"/>
+      <c r="F44" s="9"/>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" s="2"/>
       <c r="B45" s="3"/>
       <c r="C45" s="4"/>
-      <c r="D45" s="32"/>
+      <c r="D45" s="22"/>
       <c r="E45" s="2"/>
       <c r="F45" s="2"/>
     </row>
@@ -3678,7 +3898,7 @@
       <c r="A46" s="2"/>
       <c r="B46" s="3"/>
       <c r="C46" s="4"/>
-      <c r="D46" s="32"/>
+      <c r="D46" s="22"/>
       <c r="E46" s="2"/>
       <c r="F46" s="2"/>
     </row>
@@ -3686,7 +3906,7 @@
       <c r="A47" s="2"/>
       <c r="B47" s="3"/>
       <c r="C47" s="4"/>
-      <c r="D47" s="32"/>
+      <c r="D47" s="22"/>
       <c r="E47" s="2"/>
       <c r="F47" s="2"/>
     </row>
@@ -3694,7 +3914,7 @@
       <c r="A48" s="2"/>
       <c r="B48" s="3"/>
       <c r="C48" s="4"/>
-      <c r="D48" s="32"/>
+      <c r="D48" s="22"/>
       <c r="E48" s="2"/>
       <c r="F48" s="2"/>
     </row>
@@ -3702,7 +3922,7 @@
       <c r="A49" s="2"/>
       <c r="B49" s="3"/>
       <c r="C49" s="4"/>
-      <c r="D49" s="32"/>
+      <c r="D49" s="22"/>
       <c r="E49" s="2"/>
       <c r="F49" s="2"/>
     </row>
@@ -3710,7 +3930,7 @@
       <c r="A50" s="2"/>
       <c r="B50" s="3"/>
       <c r="C50" s="4"/>
-      <c r="D50" s="32"/>
+      <c r="D50" s="22"/>
       <c r="E50" s="2"/>
       <c r="F50" s="2"/>
     </row>
@@ -3718,7 +3938,7 @@
       <c r="A51" s="2"/>
       <c r="B51" s="3"/>
       <c r="C51" s="4"/>
-      <c r="D51" s="32"/>
+      <c r="D51" s="22"/>
       <c r="E51" s="2"/>
       <c r="F51" s="2"/>
     </row>
@@ -3726,7 +3946,7 @@
       <c r="A52" s="2"/>
       <c r="B52" s="3"/>
       <c r="C52" s="4"/>
-      <c r="D52" s="32"/>
+      <c r="D52" s="22"/>
       <c r="E52" s="2"/>
       <c r="F52" s="2"/>
     </row>
@@ -3744,6 +3964,7 @@
     <mergeCell ref="F1:F2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3765,82 +3986,82 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="36" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="37" t="s">
         <v>103</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="36" t="s">
         <v>52</v>
       </c>
-      <c r="D1" s="24" t="s">
+      <c r="D1" s="30" t="s">
         <v>178</v>
       </c>
-      <c r="E1" s="24" t="s">
+      <c r="E1" s="30" t="s">
         <v>179</v>
       </c>
-      <c r="F1" s="24" t="s">
+      <c r="F1" s="30" t="s">
         <v>180</v>
       </c>
-      <c r="G1" s="24" t="s">
+      <c r="G1" s="30" t="s">
         <v>181</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="14"/>
-      <c r="B2" s="15"/>
-      <c r="C2" s="14"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="25"/>
+      <c r="A2" s="36"/>
+      <c r="B2" s="37"/>
+      <c r="C2" s="36"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="31"/>
+      <c r="G2" s="31"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="4"/>
       <c r="B3" s="5"/>
-      <c r="C3" s="16"/>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16"/>
-      <c r="F3" s="16"/>
-      <c r="G3" s="17"/>
+      <c r="C3" s="12"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="12"/>
+      <c r="G3" s="13"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="4"/>
       <c r="B4" s="5"/>
-      <c r="C4" s="11"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
-      <c r="F4" s="11"/>
-      <c r="G4" s="18"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="14"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="4"/>
       <c r="B5" s="5"/>
-      <c r="C5" s="11"/>
-      <c r="D5" s="11"/>
-      <c r="E5" s="19"/>
-      <c r="F5" s="11"/>
-      <c r="G5" s="18"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="15"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="14"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="4">
         <v>4</v>
       </c>
       <c r="B6" s="5"/>
-      <c r="C6" s="11" t="s">
+      <c r="C6" s="9" t="s">
         <v>115</v>
       </c>
-      <c r="D6" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="E6" s="11" t="s">
+      <c r="D6" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="E6" s="9" t="s">
         <v>116</v>
       </c>
-      <c r="F6" s="11" t="s">
-        <v>107</v>
-      </c>
-      <c r="G6" s="18" t="s">
+      <c r="F6" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="G6" s="14" t="s">
         <v>117</v>
       </c>
     </row>
@@ -3849,19 +4070,19 @@
         <v>5</v>
       </c>
       <c r="B7" s="5"/>
-      <c r="C7" s="11" t="s">
+      <c r="C7" s="9" t="s">
         <v>118</v>
       </c>
-      <c r="D7" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="E7" s="11" t="s">
+      <c r="D7" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="E7" s="9" t="s">
         <v>119</v>
       </c>
-      <c r="F7" s="11" t="s">
-        <v>107</v>
-      </c>
-      <c r="G7" s="12" t="s">
+      <c r="F7" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="G7" s="10" t="s">
         <v>120</v>
       </c>
     </row>
@@ -3870,49 +4091,49 @@
         <v>6</v>
       </c>
       <c r="B8" s="5"/>
-      <c r="C8" s="11" t="s">
+      <c r="C8" s="9" t="s">
         <v>121</v>
       </c>
-      <c r="D8" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="E8" s="11" t="s">
+      <c r="D8" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="E8" s="9" t="s">
         <v>122</v>
       </c>
-      <c r="F8" s="11" t="s">
-        <v>107</v>
-      </c>
-      <c r="G8" s="12" t="s">
+      <c r="F8" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="G8" s="10" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="4"/>
       <c r="B9" s="5"/>
-      <c r="C9" s="11"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="12"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="10"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="4">
         <v>8</v>
       </c>
       <c r="B10" s="5"/>
-      <c r="C10" s="11" t="s">
+      <c r="C10" s="9" t="s">
         <v>127</v>
       </c>
-      <c r="D10" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="E10" s="11" t="s">
+      <c r="D10" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="E10" s="9" t="s">
         <v>128</v>
       </c>
-      <c r="F10" s="11" t="s">
-        <v>107</v>
-      </c>
-      <c r="G10" s="12" t="s">
+      <c r="F10" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="G10" s="10" t="s">
         <v>129</v>
       </c>
     </row>
@@ -3921,49 +4142,49 @@
         <v>9</v>
       </c>
       <c r="B11" s="5"/>
-      <c r="C11" s="11" t="s">
+      <c r="C11" s="9" t="s">
         <v>130</v>
       </c>
-      <c r="D11" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="E11" s="11" t="s">
+      <c r="D11" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="E11" s="9" t="s">
         <v>131</v>
       </c>
-      <c r="F11" s="11" t="s">
-        <v>107</v>
-      </c>
-      <c r="G11" s="12" t="s">
+      <c r="F11" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="G11" s="10" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="4"/>
       <c r="B12" s="5"/>
-      <c r="C12" s="11"/>
-      <c r="D12" s="11"/>
-      <c r="E12" s="11"/>
-      <c r="F12" s="11"/>
-      <c r="G12" s="18"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="9"/>
+      <c r="G12" s="14"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="4">
         <v>11</v>
       </c>
       <c r="B13" s="5"/>
-      <c r="C13" s="11" t="s">
+      <c r="C13" s="9" t="s">
         <v>136</v>
       </c>
-      <c r="D13" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="E13" s="11" t="s">
+      <c r="D13" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="E13" s="9" t="s">
         <v>137</v>
       </c>
-      <c r="F13" s="11" t="s">
-        <v>107</v>
-      </c>
-      <c r="G13" s="12" t="s">
+      <c r="F13" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="G13" s="10" t="s">
         <v>138</v>
       </c>
     </row>
@@ -3972,19 +4193,19 @@
         <v>12</v>
       </c>
       <c r="B14" s="5"/>
-      <c r="C14" s="11" t="s">
+      <c r="C14" s="9" t="s">
         <v>139</v>
       </c>
-      <c r="D14" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="E14" s="11" t="s">
+      <c r="D14" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="E14" s="9" t="s">
         <v>140</v>
       </c>
-      <c r="F14" s="11" t="s">
-        <v>107</v>
-      </c>
-      <c r="G14" s="12" t="s">
+      <c r="F14" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="G14" s="10" t="s">
         <v>141</v>
       </c>
     </row>
@@ -3993,19 +4214,19 @@
         <v>13</v>
       </c>
       <c r="B15" s="5"/>
-      <c r="C15" s="11" t="s">
+      <c r="C15" s="9" t="s">
         <v>142</v>
       </c>
-      <c r="D15" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="E15" s="11" t="s">
+      <c r="D15" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="E15" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="F15" s="11" t="s">
-        <v>107</v>
-      </c>
-      <c r="G15" s="11" t="s">
+      <c r="F15" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="G15" s="9" t="s">
         <v>144</v>
       </c>
     </row>
@@ -4014,19 +4235,19 @@
         <v>14</v>
       </c>
       <c r="B16" s="5"/>
-      <c r="C16" s="11" t="s">
+      <c r="C16" s="9" t="s">
         <v>145</v>
       </c>
-      <c r="D16" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="E16" s="11" t="s">
+      <c r="D16" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="E16" s="9" t="s">
         <v>146</v>
       </c>
-      <c r="F16" s="11" t="s">
-        <v>107</v>
-      </c>
-      <c r="G16" s="11" t="s">
+      <c r="F16" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="G16" s="9" t="s">
         <v>147</v>
       </c>
     </row>
@@ -4035,19 +4256,19 @@
         <v>15</v>
       </c>
       <c r="B17" s="5"/>
-      <c r="C17" s="11" t="s">
+      <c r="C17" s="9" t="s">
         <v>148</v>
       </c>
-      <c r="D17" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="E17" s="11" t="s">
+      <c r="D17" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="E17" s="9" t="s">
         <v>149</v>
       </c>
-      <c r="F17" s="11" t="s">
-        <v>107</v>
-      </c>
-      <c r="G17" s="11" t="s">
+      <c r="F17" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="G17" s="9" t="s">
         <v>150</v>
       </c>
     </row>
@@ -4056,19 +4277,19 @@
         <v>16</v>
       </c>
       <c r="B18" s="5"/>
-      <c r="C18" s="11" t="s">
+      <c r="C18" s="9" t="s">
         <v>151</v>
       </c>
-      <c r="D18" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="E18" s="11" t="s">
+      <c r="D18" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="E18" s="9" t="s">
         <v>152</v>
       </c>
-      <c r="F18" s="11" t="s">
-        <v>107</v>
-      </c>
-      <c r="G18" s="11" t="s">
+      <c r="F18" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="G18" s="9" t="s">
         <v>153</v>
       </c>
     </row>
@@ -4077,19 +4298,19 @@
         <v>17</v>
       </c>
       <c r="B19" s="5"/>
-      <c r="C19" s="11" t="s">
+      <c r="C19" s="9" t="s">
         <v>154</v>
       </c>
-      <c r="D19" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="E19" s="11" t="s">
+      <c r="D19" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="E19" s="9" t="s">
         <v>155</v>
       </c>
-      <c r="F19" s="11" t="s">
-        <v>107</v>
-      </c>
-      <c r="G19" s="11" t="s">
+      <c r="F19" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="G19" s="9" t="s">
         <v>156</v>
       </c>
     </row>
@@ -4098,19 +4319,19 @@
         <v>18</v>
       </c>
       <c r="B20" s="5"/>
-      <c r="C20" s="11" t="s">
+      <c r="C20" s="9" t="s">
         <v>157</v>
       </c>
-      <c r="D20" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="E20" s="11" t="s">
+      <c r="D20" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="E20" s="9" t="s">
         <v>158</v>
       </c>
-      <c r="F20" s="11" t="s">
-        <v>107</v>
-      </c>
-      <c r="G20" s="11" t="s">
+      <c r="F20" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="G20" s="9" t="s">
         <v>159</v>
       </c>
     </row>
@@ -4119,19 +4340,19 @@
         <v>19</v>
       </c>
       <c r="B21" s="5"/>
-      <c r="C21" s="11" t="s">
+      <c r="C21" s="9" t="s">
         <v>160</v>
       </c>
-      <c r="D21" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="E21" s="11" t="s">
+      <c r="D21" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="E21" s="9" t="s">
         <v>161</v>
       </c>
-      <c r="F21" s="11" t="s">
-        <v>107</v>
-      </c>
-      <c r="G21" s="11" t="s">
+      <c r="F21" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="G21" s="9" t="s">
         <v>162</v>
       </c>
     </row>
@@ -4140,19 +4361,19 @@
         <v>20</v>
       </c>
       <c r="B22" s="5"/>
-      <c r="C22" s="11" t="s">
+      <c r="C22" s="9" t="s">
         <v>163</v>
       </c>
-      <c r="D22" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="E22" s="11" t="s">
+      <c r="D22" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="E22" s="9" t="s">
         <v>164</v>
       </c>
-      <c r="F22" s="11" t="s">
-        <v>107</v>
-      </c>
-      <c r="G22" s="11" t="s">
+      <c r="F22" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="G22" s="9" t="s">
         <v>165</v>
       </c>
     </row>
@@ -4161,19 +4382,19 @@
         <v>21</v>
       </c>
       <c r="B23" s="5"/>
-      <c r="C23" s="11" t="s">
+      <c r="C23" s="9" t="s">
         <v>166</v>
       </c>
-      <c r="D23" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="E23" s="11" t="s">
+      <c r="D23" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="E23" s="9" t="s">
         <v>167</v>
       </c>
-      <c r="F23" s="11" t="s">
-        <v>107</v>
-      </c>
-      <c r="G23" s="11" t="s">
+      <c r="F23" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="G23" s="9" t="s">
         <v>168</v>
       </c>
     </row>
@@ -4182,19 +4403,19 @@
         <v>22</v>
       </c>
       <c r="B24" s="5"/>
-      <c r="C24" s="11" t="s">
+      <c r="C24" s="9" t="s">
         <v>169</v>
       </c>
-      <c r="D24" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="E24" s="11" t="s">
+      <c r="D24" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="E24" s="9" t="s">
         <v>170</v>
       </c>
-      <c r="F24" s="11" t="s">
-        <v>107</v>
-      </c>
-      <c r="G24" s="11" t="s">
+      <c r="F24" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="G24" s="9" t="s">
         <v>171</v>
       </c>
     </row>
@@ -4203,19 +4424,19 @@
         <v>23</v>
       </c>
       <c r="B25" s="5"/>
-      <c r="C25" s="11" t="s">
+      <c r="C25" s="9" t="s">
         <v>172</v>
       </c>
-      <c r="D25" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="E25" s="11" t="s">
+      <c r="D25" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="E25" s="9" t="s">
         <v>173</v>
       </c>
-      <c r="F25" s="11" t="s">
-        <v>107</v>
-      </c>
-      <c r="G25" s="11" t="s">
+      <c r="F25" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="G25" s="9" t="s">
         <v>174</v>
       </c>
     </row>
@@ -4224,19 +4445,19 @@
         <v>24</v>
       </c>
       <c r="B26" s="5"/>
-      <c r="C26" s="11" t="s">
+      <c r="C26" s="9" t="s">
         <v>175</v>
       </c>
-      <c r="D26" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="E26" s="11" t="s">
+      <c r="D26" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="E26" s="9" t="s">
         <v>176</v>
       </c>
-      <c r="F26" s="11" t="s">
-        <v>107</v>
-      </c>
-      <c r="G26" s="11" t="s">
+      <c r="F26" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="G26" s="9" t="s">
         <v>177</v>
       </c>
     </row>
@@ -4257,7 +4478,7 @@
       <c r="F27" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="G27" s="20" t="s">
+      <c r="G27" s="16" t="s">
         <v>184</v>
       </c>
     </row>
@@ -4278,7 +4499,7 @@
       <c r="F28" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="G28" s="20" t="s">
+      <c r="G28" s="16" t="s">
         <v>186</v>
       </c>
     </row>
@@ -4293,13 +4514,13 @@
       <c r="D29" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="E29" s="21" t="s">
+      <c r="E29" s="17" t="s">
         <v>188</v>
       </c>
       <c r="F29" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="G29" s="20" t="s">
+      <c r="G29" s="16" t="s">
         <v>189</v>
       </c>
     </row>
@@ -4314,13 +4535,13 @@
       <c r="D30" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="E30" s="21" t="s">
+      <c r="E30" s="17" t="s">
         <v>193</v>
       </c>
       <c r="F30" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="G30" s="20" t="s">
+      <c r="G30" s="16" t="s">
         <v>192</v>
       </c>
     </row>
@@ -4335,13 +4556,13 @@
       <c r="D31" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="E31" s="21" t="s">
+      <c r="E31" s="17" t="s">
         <v>196</v>
       </c>
-      <c r="F31" s="22" t="s">
+      <c r="F31" s="18" t="s">
         <v>195</v>
       </c>
-      <c r="G31" s="23" t="s">
+      <c r="G31" s="19" t="s">
         <v>197</v>
       </c>
     </row>

</xml_diff>